<commit_message>
json schema of mock user
</commit_message>
<xml_diff>
--- a/src/main/java/com/Datasheet/RingPayAPI_TestData_stage.xlsx
+++ b/src/main/java/com/Datasheet/RingPayAPI_TestData_stage.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="841">
   <si>
     <t>TestCases</t>
   </si>
@@ -2536,6 +2536,27 @@
   </si>
   <si>
     <t>4202055.0</t>
+  </si>
+  <si>
+    <t>6818087119</t>
+  </si>
+  <si>
+    <t>Niyati</t>
+  </si>
+  <si>
+    <t>KailashRaja65125@example.net</t>
+  </si>
+  <si>
+    <t>1989-01-26</t>
+  </si>
+  <si>
+    <t>752745609345715</t>
+  </si>
+  <si>
+    <t>IDEP6169959956125LUT</t>
+  </si>
+  <si>
+    <t>4202069.0</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3037,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -3168,7 +3189,7 @@
         <v>888888</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -3185,7 +3206,7 @@
         <v>125111</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -3202,7 +3223,7 @@
         <v>555555</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -3219,7 +3240,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -3236,7 +3257,7 @@
         <v>789</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -3305,7 +3326,7 @@
         <v>82</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="F2" s="19">
         <v>18.939800000000002</v>
@@ -3535,7 +3556,7 @@
         <v>82</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>72</v>
@@ -3692,7 +3713,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>109</v>
@@ -3876,13 +3897,13 @@
         <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="F2" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>31</v>
@@ -4217,10 +4238,10 @@
         <v>56</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="E2" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>69</v>
@@ -4232,7 +4253,7 @@
         <v>71</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>72</v>
@@ -4241,10 +4262,10 @@
         <v>73</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c r="M2" s="17" t="n">
-        <v>4202069.0</v>
+        <v>4202229.0</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>74</v>

</xml_diff>